<commit_message>
Update Arbeidsmarkedstilknytning for Vestfold kommuner og hele landet 2023 SSB 13563.xlsx
</commit_message>
<xml_diff>
--- a/03_Arbeid og næringsliv/Sysselsetting/2023/Arbeidsmarkedstilknytning for Vestfold kommuner og hele landet 2023 SSB 13563.xlsx
+++ b/03_Arbeid og næringsliv/Sysselsetting/2023/Arbeidsmarkedstilknytning for Vestfold kommuner og hele landet 2023 SSB 13563.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vestfoldfylke-my.sharepoint.com/personal/ellen_just_hansen_vestfoldfylke_no/Documents/Dokumenter/GitHub/Nyeste Github versjon/Vestfold/03_Arbeid og næringsliv/Sysselsetting/2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="8_{092C5882-4963-4F00-8A4A-9F1959421224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85156DA6-A188-4FB6-8399-B0D6133406C4}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="8_{092C5882-4963-4F00-8A4A-9F1959421224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99F76985-A44B-4028-B56B-54EB1F25A997}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bosatte" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>2023</t>
   </si>
@@ -90,6 +90,21 @@
   </si>
   <si>
     <t>Prosent</t>
+  </si>
+  <si>
+    <t>Arbeidsledige</t>
+  </si>
+  <si>
+    <t>Arbeidsmarkedstiltak</t>
+  </si>
+  <si>
+    <t>Utdanning</t>
+  </si>
+  <si>
+    <t>AAP / uføretrygd</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AFP/alderspensjon</t>
   </si>
 </sst>
 </file>
@@ -97,7 +112,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0\ %"/>
+    <numFmt numFmtId="164" formatCode="0.0\ %"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -152,9 +167,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,7 +476,7 @@
   <dimension ref="A3:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -758,19 +773,19 @@
         <v>3</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>9</v>
@@ -946,7 +961,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="5">
-        <f t="shared" si="0"/>
+        <f>(C11/B11)</f>
         <v>0.58144951610573448</v>
       </c>
       <c r="D23" s="5">

</xml_diff>